<commit_message>
OMU-1937 User Model Registration
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/RegistrationTestData.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/RegistrationTestData.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6052AFAF-A5A2-47CB-B7AD-34D8BEA6C15A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Raj\git\nordsonomu_automation\nordson.omu\nordson.omu\src\test\java\com\nordson\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE635D64-34F8-46AA-810F-6EF924CA7764}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17304" windowHeight="12384" xr2:uid="{8C11D641-32A4-4541-BB63-F9C6450806B5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8C11D641-32A4-4541-BB63-F9C6450806B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>First Name</t>
   </si>
@@ -47,12 +51,6 @@
     <t>Desc</t>
   </si>
   <si>
-    <t>EmailAddress</t>
-  </si>
-  <si>
-    <t>ConfirmEmailAddress</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -78,16 +76,13 @@
   </si>
   <si>
     <t>Test1234567</t>
-  </si>
-  <si>
-    <t>ravitest68@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,14 +101,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,11 +144,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -169,10 +155,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -485,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80478CC2-5625-4CDC-B21E-8C48D032A7A6}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,13 +485,11 @@
     <col min="6" max="6" width="17.88671875" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="16.77734375" customWidth="1"/>
-    <col min="9" max="9" width="27.44140625" customWidth="1"/>
-    <col min="10" max="10" width="34.88671875" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="12" max="12" width="27.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,58 +520,42 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="E2" s="2">
         <v>988272727</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G2" s="4">
         <v>8546001</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{50094C79-0401-4376-B738-3C5A84A4F6BE}"/>
-    <hyperlink ref="J2" r:id="rId2" xr:uid="{E88E4959-5BE2-4A66-BE9A-6849976C3001}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>